<commit_message>
Anpassung für Excel Export der Gruppen
</commit_message>
<xml_diff>
--- a/LagerInsights/Resources/Vorlagen/Gruppendaten.xlsx
+++ b/LagerInsights/Resources/Vorlagen/Gruppendaten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\kzl-teilnehmenden-auswertung\BWB-Auswertung\Resources\Vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\kzl-teilnehmenden-auswertung\LagerInsights\Resources\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F074A05D-AF8F-4C26-9098-B92238F38DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597628EF-3A67-4949-8081-D34BAB0DD98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="38700" windowHeight="15345" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,49 +36,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>OU</t>
-  </si>
-  <si>
-    <t>Feuerwehr</t>
-  </si>
-  <si>
-    <t>Geschlecht</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Vorname</t>
   </si>
   <si>
-    <t>Nachname</t>
-  </si>
-  <si>
     <t>Alter</t>
   </si>
   <si>
-    <t>Gruppendaten</t>
-  </si>
-  <si>
     <t>Geburtsdatum</t>
   </si>
   <si>
-    <t>LagerNr</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Essgewohnheiten</t>
   </si>
   <si>
     <t>Unverträglichkeiten</t>
+  </si>
+  <si>
+    <t>Verbindliche Teilnehmende für das Zeltlager</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Jugendfeuerwehr</t>
+  </si>
+  <si>
+    <t>PLZ</t>
+  </si>
+  <si>
+    <t>Ort</t>
+  </si>
+  <si>
+    <t>M/W/D/N</t>
+  </si>
+  <si>
+    <t>Organisationseinheit</t>
+  </si>
+  <si>
+    <t>Straße, Hausnummer</t>
+  </si>
+  <si>
+    <t>TN Status</t>
+  </si>
+  <si>
+    <t>Zu überweisen</t>
+  </si>
+  <si>
+    <t>Bereits überwiesen</t>
+  </si>
+  <si>
+    <t>Anzahl an Teilnehmdenen:</t>
+  </si>
+  <si>
+    <t>Davon Vegetrarier:</t>
+  </si>
+  <si>
+    <t>Davon Veganer:</t>
+  </si>
+  <si>
+    <t>Davon mit besonderen Essgewohnheiten:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,7 +119,15 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,14 +150,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -141,6 +224,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEEB4737-25EB-40FE-BFA5-987D0BC33B50}" name="Tabelle1" displayName="Tabelle1" ref="A10:O11" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A10:O11" xr:uid="{CEEB4737-25EB-40FE-BFA5-987D0BC33B50}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{A9F970DE-D1B6-4EAC-AEE5-10DEBFE983B2}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{CF6F5905-4378-40BC-9726-5DCBC501E6A1}" name="Vorname"/>
+    <tableColumn id="15" xr3:uid="{C1E5D8A1-494F-4390-AD17-0DDEAFA3EE07}" name="Geburtsdatum"/>
+    <tableColumn id="3" xr3:uid="{8A46AC37-CF56-4A32-A9BD-5CFD4F21BD8A}" name="Alter"/>
+    <tableColumn id="4" xr3:uid="{68C2EA5E-3E5B-4618-B588-8999E29E7125}" name="M/W/D/N"/>
+    <tableColumn id="5" xr3:uid="{187D3649-CA1D-4B16-AD26-88E0C99FDF52}" name="PLZ"/>
+    <tableColumn id="6" xr3:uid="{B499CCD4-5812-45FD-B3EC-B60BF3F60B34}" name="Ort"/>
+    <tableColumn id="7" xr3:uid="{F53B9BDC-CE5C-4479-9230-E737A3297357}" name="Straße, Hausnummer"/>
+    <tableColumn id="8" xr3:uid="{EC304FE3-F975-488C-A380-85E7FD0029AF}" name="TN Status"/>
+    <tableColumn id="9" xr3:uid="{F85E1D65-DF69-4E68-A9BE-769B1CA1114B}" name="Jugendfeuerwehr"/>
+    <tableColumn id="10" xr3:uid="{2EA8FF55-5513-4C6B-B5C7-D4E0D8AE1511}" name="Organisationseinheit"/>
+    <tableColumn id="11" xr3:uid="{BC90830D-9E89-45E1-813E-7C006B1CF668}" name="Essgewohnheiten"/>
+    <tableColumn id="12" xr3:uid="{369BBB8B-7A0E-4CB2-A827-FA9F395FA013}" name="Unverträglichkeiten"/>
+    <tableColumn id="13" xr3:uid="{30E398A4-BF6E-428B-8329-0620A1EA1984}" name="Zu überweisen"/>
+    <tableColumn id="14" xr3:uid="{059B739E-DAB5-463F-BCCD-8B0EE4045373}" name="Bereits überwiesen"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,68 +547,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2D032-C0E4-4A24-9496-66E6E37D5C8D}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="45.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.85546875" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:15" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <f>SUM(Tabelle1[Name])</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="9">
+        <f>SUM(Tabelle1[Vorname])</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <f>SUM(Tabelle1[Geburtsdatum])</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <f>SUM(Tabelle1[Alter])</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <f>SUM(Tabelle1[M/W/D/N])</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <f>SUM(Tabelle1[PLZ])</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <f>SUM(Tabelle1[Ort])</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <f>SUM(Tabelle1[Straße, Hausnummer])</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <f>SUM(Tabelle1[TN Status])</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <f>SUM(Tabelle1[Jugendfeuerwehr])</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <f>SUM(Tabelle1[Organisationseinheit])</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <f>SUM(Tabelle1[Essgewohnheiten])</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <f>SUM(Tabelle1[Unverträglichkeiten])</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <f>SUM(Tabelle1[Zu überweisen])</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <f>SUM(Tabelle1[Bereits überwiesen])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="M10" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anzahl Teilnehmer in Essensliste
</commit_message>
<xml_diff>
--- a/LagerInsights/Resources/Vorlagen/Gruppendaten.xlsx
+++ b/LagerInsights/Resources/Vorlagen/Gruppendaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\kzl-teilnehmenden-auswertung\LagerInsights\Resources\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597628EF-3A67-4949-8081-D34BAB0DD98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE87E858-88DD-40E2-8331-237D76D3C136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Vorname</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Davon mit besonderen Essgewohnheiten:</t>
+  </si>
+  <si>
+    <t>Anzahl Teilnehmer bei aktuellem Filter:</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,6 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -199,14 +201,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -550,14 +553,13 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" customWidth="1"/>
@@ -579,97 +581,62 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="9"/>
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5">
+        <f>ROWS(Tabelle1[])</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <f>SUM(Tabelle1[Name])</f>
-        <v>0</v>
-      </c>
-      <c r="B9" s="9">
-        <f>SUM(Tabelle1[Vorname])</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <f>SUM(Tabelle1[Geburtsdatum])</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <f>SUM(Tabelle1[Alter])</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
-        <f>SUM(Tabelle1[M/W/D/N])</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <f>SUM(Tabelle1[PLZ])</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <f>SUM(Tabelle1[Ort])</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <f>SUM(Tabelle1[Straße, Hausnummer])</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <f>SUM(Tabelle1[TN Status])</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
-        <f>SUM(Tabelle1[Jugendfeuerwehr])</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <f>SUM(Tabelle1[Organisationseinheit])</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="9">
-        <f>SUM(Tabelle1[Essgewohnheiten])</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <f>SUM(Tabelle1[Unverträglichkeiten])</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="9">
-        <f>SUM(Tabelle1[Zu überweisen])</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="9">
-        <f>SUM(Tabelle1[Bereits überwiesen])</f>
-        <v>0</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -678,7 +645,7 @@
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">

</xml_diff>

<commit_message>
Upload der Gruppendaten zurück auf den Webserver
Und prüfen der Änderungen
</commit_message>
<xml_diff>
--- a/LagerInsights/Resources/Vorlagen/Gruppendaten.xlsx
+++ b/LagerInsights/Resources/Vorlagen/Gruppendaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\kzl-teilnehmenden-auswertung\LagerInsights\Resources\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE87E858-88DD-40E2-8331-237D76D3C136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D776D900-66F8-4128-AA47-57E0D7AE43AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Vorname</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Anzahl Teilnehmer bei aktuellem Filter:</t>
+  </si>
+  <si>
+    <t>Unterlagen vorhanden</t>
+  </si>
+  <si>
+    <t>Zeltdorf</t>
   </si>
 </sst>
 </file>
@@ -209,7 +215,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -230,9 +236,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEEB4737-25EB-40FE-BFA5-987D0BC33B50}" name="Tabelle1" displayName="Tabelle1" ref="A10:O11" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A10:O11" xr:uid="{CEEB4737-25EB-40FE-BFA5-987D0BC33B50}"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEEB4737-25EB-40FE-BFA5-987D0BC33B50}" name="Tabelle1" displayName="Tabelle1" ref="A10:Q11" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A10:Q11" xr:uid="{CEEB4737-25EB-40FE-BFA5-987D0BC33B50}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{A9F970DE-D1B6-4EAC-AEE5-10DEBFE983B2}" name="Name"/>
     <tableColumn id="2" xr3:uid="{CF6F5905-4378-40BC-9726-5DCBC501E6A1}" name="Vorname"/>
     <tableColumn id="15" xr3:uid="{C1E5D8A1-494F-4390-AD17-0DDEAFA3EE07}" name="Geburtsdatum"/>
@@ -248,6 +254,8 @@
     <tableColumn id="12" xr3:uid="{369BBB8B-7A0E-4CB2-A827-FA9F395FA013}" name="Unverträglichkeiten"/>
     <tableColumn id="13" xr3:uid="{30E398A4-BF6E-428B-8329-0620A1EA1984}" name="Zu überweisen"/>
     <tableColumn id="14" xr3:uid="{059B739E-DAB5-463F-BCCD-8B0EE4045373}" name="Bereits überwiesen"/>
+    <tableColumn id="16" xr3:uid="{6FE0EF79-F25A-44CA-854A-2111E7D6AAC1}" name="Unterlagen vorhanden"/>
+    <tableColumn id="17" xr3:uid="{B4B6D845-DC26-4D02-B818-6E2C5DB2D7FF}" name="Zeltdorf"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -550,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2D032-C0E4-4A24-9496-66E6E37D5C8D}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,15 +580,17 @@
     <col min="13" max="13" width="35.42578125" customWidth="1"/>
     <col min="14" max="14" width="22.5703125" customWidth="1"/>
     <col min="15" max="15" width="28.140625" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:17" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -589,8 +599,8 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -611,8 +621,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -621,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -638,7 +648,7 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -683,6 +693,12 @@
       </c>
       <c r="O10" t="s">
         <v>15</v>
+      </c>
+      <c r="P10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>